<commit_message>
split code into classes
</commit_message>
<xml_diff>
--- a/old_worklist.xlsx
+++ b/old_worklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabewilson/Desktop/worklist_generation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F026D38-F8BA-F343-A702-5DA5F29754F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76ABFD78-F0C6-2D43-B467-8C668FE58E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17080" xr2:uid="{BF50EA0A-2797-EC49-8565-645DB7B38C61}"/>
   </bookViews>
@@ -1038,9 +1038,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79332BF3-487A-D048-AE38-CBE359952258}">
   <dimension ref="A1:AS58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH53" sqref="AH53"/>
+      <selection pane="bottomLeft" activeCell="AH23" sqref="AH23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>